<commit_message>
added xml file to run suite test
</commit_message>
<xml_diff>
--- a/TestNGClassTest/src/test/resources/Files/testdata.xlsx
+++ b/TestNGClassTest/src/test/resources/Files/testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17" count="2">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1350,13 +1350,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="45" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6719" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="45.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="25.5" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="12.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.5" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="32.5" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="20.6719" collapsed="false"/>
+    <col min="7" max="16384" customWidth="true" style="1" width="8.85156" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">

</xml_diff>